<commit_message>
init board added to test cases
</commit_message>
<xml_diff>
--- a/TO DELETE LATER/Board.xlsx
+++ b/TO DELETE LATER/Board.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ludo_SMG\TO DELETE LATER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkunaparaju\Documents\GitHub\Ludo_SMG\TO DELETE LATER\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -606,7 +606,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>